<commit_message>
Add Anforderungen and update Grundlagen
</commit_message>
<xml_diff>
--- a/Recherche/ThreadObjekte.xlsx
+++ b/Recherche/ThreadObjekte.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24606"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="120" documentId="11_92483E2D04E89AD36523F29B863E8C1851038389" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59A11AA1-331D-49C5-9261-A1F1F995A65C}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ec6cc8aaa6ec186/OTH/Master/MI4/Masterarbeit/Recherche/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="122" documentId="11_92483E2D04E89AD36523F29B863E8C1851038389" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{352BA458-A666-4D2B-A7AB-971B89E982B5}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -170,7 +175,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,7 +224,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -518,16 +523,16 @@
   <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,7 +540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -543,7 +548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -551,7 +556,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -559,7 +564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -567,7 +572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -575,7 +580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -583,7 +588,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -591,7 +596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -599,7 +604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -607,7 +612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -615,7 +620,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -623,7 +628,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -631,7 +636,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -639,7 +644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -647,7 +652,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -655,7 +660,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -663,7 +668,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -671,7 +676,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -679,7 +684,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -687,7 +692,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -695,7 +700,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -703,7 +708,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -711,7 +716,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -719,7 +724,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -727,7 +732,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -735,7 +740,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -743,7 +748,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -751,7 +756,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -759,7 +764,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -767,7 +772,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -775,7 +780,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -783,7 +788,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -791,7 +796,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -799,7 +804,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -807,7 +812,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -815,7 +820,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -823,7 +828,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -831,7 +836,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -839,7 +844,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -847,7 +852,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -855,7 +860,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -863,7 +868,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -871,7 +876,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -879,7 +884,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -887,7 +892,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -895,7 +900,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -903,7 +908,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -911,7 +916,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -919,7 +924,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -927,7 +932,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -935,7 +940,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -943,7 +948,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -958,5 +963,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>